<commit_message>
add ErrorColumns & fix errors
</commit_message>
<xml_diff>
--- a/static/uploads/dataTest_with_error.xlsx
+++ b/static/uploads/dataTest_with_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\YoProgramo\python\Api_FastAPI\exel_to_database\static\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED589BC-264A-4670-90D8-7AF94FE7E444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DDDA62-2D50-4E93-8340-69F9ED4A6DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4875" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{FCE606B2-40F1-469F-A927-FD75F1CDBDAF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>adri@gmail.com</t>
   </si>
   <si>
-    <t>Adri</t>
-  </si>
-  <si>
     <t>Parra</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>gh</t>
-  </si>
-  <si>
     <t>Matias</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>tintin@outlook.com.ar</t>
   </si>
   <si>
-    <t>alan@gmail.com</t>
-  </si>
-  <si>
     <t>more@hotmail.com</t>
   </si>
   <si>
@@ -121,6 +109,12 @@
   </si>
   <si>
     <t>nico95@outlook.com.ar</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>456456@</t>
   </si>
 </sst>
 </file>
@@ -195,12 +189,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -519,7 +514,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +537,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,13 +545,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -570,27 +565,27 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>21412</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>234</v>
@@ -601,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -618,13 +613,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E6">
         <v>234</v>
@@ -638,30 +633,30 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>453453</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8">
-        <v>43534</v>
+        <v>4353</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,13 +664,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E9">
         <v>34534</v>
@@ -686,13 +681,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E10">
         <v>3534</v>
@@ -706,24 +701,27 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>634</v>

</xml_diff>